<commit_message>
Cargue de versiones finales
</commit_message>
<xml_diff>
--- a/resultado_transcripciones.xlsx
+++ b/resultado_transcripciones.xlsx
@@ -505,7 +505,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -764,7 +764,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1134,7 +1134,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H50" t="n">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H53" t="n">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H57" t="n">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H64" t="n">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H65" t="n">
@@ -3169,7 +3169,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H74" t="n">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H75" t="n">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H86" t="n">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H89" t="n">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>JPY</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H111" t="n">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H113" t="n">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -4908,7 +4908,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H121" t="n">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H130" t="n">
@@ -5315,7 +5315,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H132" t="n">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H135" t="n">
@@ -5463,7 +5463,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H136" t="n">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -6129,7 +6129,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H157" t="n">
@@ -6388,7 +6388,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H161" t="n">
@@ -6647,7 +6647,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H168" t="n">
@@ -6832,7 +6832,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H173" t="n">
@@ -6906,7 +6906,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H175" t="n">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H177" t="n">
@@ -7017,7 +7017,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H178" t="n">
@@ -7128,7 +7128,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H181" t="n">
@@ -7165,7 +7165,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H182" t="n">
@@ -7350,7 +7350,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H187" t="n">
@@ -7424,7 +7424,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H189" t="n">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H192" t="n">
@@ -7609,7 +7609,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H194" t="n">
@@ -7646,7 +7646,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H195" t="n">
@@ -7720,7 +7720,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H197" t="n">
@@ -7868,7 +7868,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H201" t="n">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H204" t="n">
@@ -8460,7 +8460,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H217" t="n">
@@ -8608,7 +8608,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H221" t="n">
@@ -8756,7 +8756,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H225" t="n">
@@ -9200,7 +9200,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H237" t="n">
@@ -9348,7 +9348,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H241" t="n">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H252" t="n">
@@ -9866,7 +9866,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H255" t="n">
@@ -10236,7 +10236,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H265" t="n">
@@ -10273,7 +10273,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H266" t="n">
@@ -10421,7 +10421,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H270" t="n">
@@ -10458,7 +10458,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H271" t="n">
@@ -10532,7 +10532,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="H273" t="n">
@@ -10540,7 +10540,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>Buenos días, habla Sara Gómez de la Mesa de Divisas, es un buen momento para conversar. Estoy revisando opciones para comprar $74,356, ¿qué condiciones tienen hoy? Esta es la mejor tasa que puedo ofrecer ahora mismo, $3,820.62. Me gustaría que revisaras si puede mejorar la propuesta. Esta es la mejor tasa que puedo ofrecer ahora mismo, $3,810.94. Si me ofrece una mejora mínima, podemos concretar la operación Con la tendencia actual del mercado, 3,801.5 es una tasa muy competitiva Si mejora la tasa en al menos 15 pesos, cerramos Le puedo ofrecer una tasa de 3,792.44 si realiza la operación en los próximos minutos Podría aceptar si ajusta la tasa a unos puntos a mi favor Podemos realizar la transacción a una tasa preferencial de 3.792.44 pesos, válida solo durante los próximos minutos De acuerdo, me parece bien la oferta, avancemos Gracias. Gracias. ¿Quieres hacer referencia? 646.</t>
+          <t>Buenos días, habla Sara Gómez de la Mesa de Divisas, es un buen momento para conversar. Estoy revisando opciones para comprar $74,356 dolares, ¿qué condiciones tienen hoy? Esta es la mejor tasa que puedo ofrecer ahora mismo, $3,820.62. Me gustaría que revisaras si puede mejorar la propuesta. Esta es la mejor tasa que puedo ofrecer ahora mismo, $3,810.94. Si me ofrece una mejora mínima, podemos concretar la operación Con la tendencia actual del mercado, 3,801.5 es una tasa muy competitiva Si mejora la tasa en al menos 15 pesos, cerramos Le puedo ofrecer una tasa de 3,792.44 si realiza la operación en los próximos minutos Podría aceptar si ajusta la tasa a unos puntos a mi favor Podemos realizar la transacción a una tasa preferencial de 3.792.44 pesos, válida solo durante los próximos minutos De acuerdo, me parece bien la oferta, avancemos Gracias. Gracias. ¿Quieres hacer referencia? 646.</t>
         </is>
       </c>
     </row>
@@ -10939,7 +10939,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H284" t="n">
@@ -11013,7 +11013,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H286" t="n">
@@ -11124,7 +11124,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H289" t="n">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H299" t="n">
@@ -11938,7 +11938,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H311" t="n">
@@ -12160,7 +12160,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H317" t="n">
@@ -12234,7 +12234,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H319" t="n">
@@ -12308,7 +12308,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H321" t="n">
@@ -12419,7 +12419,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H324" t="n">
@@ -12678,7 +12678,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H331" t="n">
@@ -12715,7 +12715,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H332" t="n">
@@ -12863,7 +12863,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H336" t="n">
@@ -13233,7 +13233,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>JPY</t>
         </is>
       </c>
       <c r="H346" t="n">
@@ -13307,7 +13307,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H348" t="n">
@@ -13418,7 +13418,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H351" t="n">
@@ -13603,7 +13603,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H356" t="n">
@@ -13677,7 +13677,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H358" t="n">
@@ -13714,7 +13714,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H359" t="n">
@@ -13899,7 +13899,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H364" t="n">
@@ -13973,7 +13973,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H366" t="n">
@@ -14010,7 +14010,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H367" t="n">
@@ -14047,7 +14047,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H368" t="n">
@@ -14195,7 +14195,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H372" t="n">
@@ -14232,7 +14232,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H373" t="n">
@@ -14639,7 +14639,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H384" t="n">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H385" t="n">
@@ -14750,7 +14750,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>JPY</t>
         </is>
       </c>
       <c r="H387" t="n">
@@ -15046,7 +15046,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H395" t="n">
@@ -15083,7 +15083,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H396" t="n">
@@ -15120,7 +15120,7 @@
       </c>
       <c r="G397" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H397" t="n">
@@ -15231,7 +15231,7 @@
       </c>
       <c r="G400" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H400" t="n">
@@ -15527,7 +15527,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H408" t="n">
@@ -15564,7 +15564,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H409" t="n">
@@ -15712,7 +15712,7 @@
       </c>
       <c r="G413" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H413" t="n">
@@ -15971,7 +15971,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H420" t="n">
@@ -16193,7 +16193,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H426" t="n">
@@ -16267,7 +16267,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H428" t="n">
@@ -16415,7 +16415,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="H432" t="n">
@@ -16563,7 +16563,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H436" t="n">
@@ -16785,7 +16785,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H442" t="n">
@@ -16970,7 +16970,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H447" t="n">
@@ -17081,7 +17081,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H450" t="n">
@@ -17192,7 +17192,7 @@
       </c>
       <c r="G453" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H453" t="n">
@@ -17377,7 +17377,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H458" t="n">
@@ -17525,7 +17525,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H462" t="n">
@@ -17673,7 +17673,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="H466" t="n">
@@ -17932,7 +17932,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H473" t="n">
@@ -18376,7 +18376,7 @@
       </c>
       <c r="G485" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H485" t="n">
@@ -18635,7 +18635,7 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H492" t="n">
@@ -18746,7 +18746,7 @@
       </c>
       <c r="G495" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="H495" t="n">
@@ -18968,7 +18968,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="H501" t="n">

</xml_diff>